<commit_message>
broad updates to data gen/retrieval process
</commit_message>
<xml_diff>
--- a/Prelim_Data/Central_Valley/Central_Valley_30_90.xlsx
+++ b/Prelim_Data/Central_Valley/Central_Valley_30_90.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/aahernes_ucdavis_edu/Documents/WORK/DahlkeLab_LAWR/Prelim_Data/Central_Valley/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_DD512CD84E9CC9B5F134EAE5CD78DD913F84360A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54EE48BF-D1CE-4D14-91EF-43211570586E}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_DD512CD84E9CC9B5F134EAE5CD78DD913F84360A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75E07FE1-8D9C-4CB6-A77C-388AEB4B8F15}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1302,12 +1302,12 @@
   <dimension ref="A1:AK82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16" customWidth="1"/>
     <col min="17" max="17" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>